<commit_message>
Added extra test points
</commit_message>
<xml_diff>
--- a/Hardware/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
+++ b/Hardware/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksa\Documents\Altium\FPGA_Module\Project Outputs for FPGA_Module\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B085F888-1594-4A06-A558-7B9FB9FAA18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28F4E977-C869-464F-9309-C2974AE7852C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{5461D050-A4BF-450D-B5C1-57397EF8237F}"/>
+    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{AFAE7B96-9D9B-4C38-8130-897373CD7A47}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-FPGA_Module" sheetId="1" r:id="rId1"/>
@@ -894,7 +894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09B0F29-2945-4363-96F1-F902566E2995}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D69D382-0A8E-4A6F-8D47-0F34F97CC4B0}">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Added 25 MHz oscillator
</commit_message>
<xml_diff>
--- a/Hardware/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
+++ b/Hardware/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksa\Documents\Altium\FPGA_Module\Project Outputs for FPGA_Module\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D5BE733-4626-4C9F-B644-48080A505A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87705C9C-7640-40E7-872B-B148749CC61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{9D1E5019-97A5-493B-8F90-7145C60DFD95}"/>
+    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{D5F3CE93-3D5B-4632-8847-1B7FFEA38F33}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-FPGA_Module" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="165">
   <si>
     <t>Comment</t>
   </si>
@@ -62,7 +62,7 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>C1, C2, C3, C78, C84</t>
+    <t>C1, C2, C3, C72, C78, C84</t>
   </si>
   <si>
     <t>GEN_C_0402</t>
@@ -254,7 +254,7 @@
     <t>DMN62D0UW</t>
   </si>
   <si>
-    <t>Q1</t>
+    <t>Q1, Q2</t>
   </si>
   <si>
     <t>GEN_SOT_323</t>
@@ -269,7 +269,7 @@
     <t>100</t>
   </si>
   <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R58</t>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R9, R10, R11, R58, R62</t>
   </si>
   <si>
     <t>GEN_R_0201</t>
@@ -284,7 +284,7 @@
     <t>4.7K</t>
   </si>
   <si>
-    <t>R12, R13, R14, R15, R16</t>
+    <t>R12, R13, R14, R15, R16, R59</t>
   </si>
   <si>
     <t>RES 4.7K OHM 1% 1/20W 0201</t>
@@ -519,6 +519,21 @@
   </si>
   <si>
     <t>595-TPS62A02DRLR</t>
+  </si>
+  <si>
+    <t>25MHz</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ECS_TXO-2016</t>
+  </si>
+  <si>
+    <t>OSC 25MHz ECS-TXO-2016</t>
+  </si>
+  <si>
+    <t>XC3163CT-ND</t>
   </si>
 </sst>
 </file>
@@ -894,8 +909,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26135FCF-F085-4769-BB4D-92757B83630D}">
-  <dimension ref="A1:F36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58049938-7909-43DA-A668-7F0EAF838422}">
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -939,7 +954,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -1219,7 +1234,7 @@
         <v>73</v>
       </c>
       <c r="E16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>74</v>
@@ -1239,7 +1254,7 @@
         <v>78</v>
       </c>
       <c r="E17" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>79</v>
@@ -1259,7 +1274,7 @@
         <v>82</v>
       </c>
       <c r="E18" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>83</v>
@@ -1619,6 +1634,26 @@
       </c>
       <c r="F36" s="2" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed 50ohm trace clearance to 5mil
</commit_message>
<xml_diff>
--- a/Hardware/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
+++ b/Hardware/FPGA_Module_Rev2/Project Outputs for FPGA_Module/BOM/Bill of Materials-FPGA_Module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksa\Documents\Altium\FPGA_Module\Project Outputs for FPGA_Module\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87705C9C-7640-40E7-872B-B148749CC61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BBAD680-7199-47CC-B3F4-39C5E9B7D93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{D5F3CE93-3D5B-4632-8847-1B7FFEA38F33}"/>
+    <workbookView xWindow="4110" yWindow="4110" windowWidth="31995" windowHeight="15435" xr2:uid="{3D7179E1-9914-4BAC-BD4D-91A907A3DACC}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-FPGA_Module" sheetId="1" r:id="rId1"/>
@@ -909,7 +909,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58049938-7909-43DA-A668-7F0EAF838422}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8DCAA2-EA15-49F6-9D71-0131514B26E5}">
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>